<commit_message>
Made download button work
</commit_message>
<xml_diff>
--- a/Marvel/Content/file/OverallClinicReport.xlsx
+++ b/Marvel/Content/file/OverallClinicReport.xlsx
@@ -29,10 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Overall view of Clinic Report</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Clinic Name</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -57,23 +53,23 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>Overall view of Clinic Report</t>
+  </si>
+  <si>
     <t>Armstrong Clinic</t>
-    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>Marvelous Clinic</t>
-    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>Clinic F</t>
-    <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,11 +85,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF00B0F0"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -106,8 +114,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -120,19 +127,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -144,12 +146,60 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1090,6 +1140,21 @@
 </externalLink>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A2:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Clinic Name" dataDxfId="6"/>
+    <tableColumn id="2" name="Upload photos" dataDxfId="5"/>
+    <tableColumn id="3" name="Verified photos" dataDxfId="4"/>
+    <tableColumn id="4" name="Uploaded This Month" dataDxfId="3"/>
+    <tableColumn id="5" name="Overall Success Rate" dataDxfId="2"/>
+    <tableColumn id="6" name="This month"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1356,10 +1421,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -1369,99 +1434,99 @@
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>116</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>102</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>11</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <f>88%</f>
         <v>0.88</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <f>73%</f>
         <v>0.73</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>103</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>102</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <f>99%</f>
         <v>0.99</v>
       </c>
-      <c r="F4" s="5" t="str">
+      <c r="F4" s="3" t="str">
         <f>"Error"</f>
         <v>Error</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <f>125</f>
         <v>125</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>86</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>11</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <f>69%</f>
         <v>0.69</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1470,6 +1535,10 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>